<commit_message>
Update dokumen Test Plan, Test Monitoring, Test Report - Cek ketersediaan
</commit_message>
<xml_diff>
--- a/test-report/Test-Bug Report - indihome (Cek Ketersediaan).xlsx
+++ b/test-report/Test-Bug Report - indihome (Cek Ketersediaan).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t xml:space="preserve">TEST REPORT </t>
   </si>
@@ -20,15 +20,21 @@
     <t>Nama Project</t>
   </si>
   <si>
-    <t>:</t>
+    <t>: Validasi Fitur-fitur Situs Indihome dengan Pengujian Otomatis Menggunakan Selenium</t>
   </si>
   <si>
     <t>Nama Fitur</t>
   </si>
   <si>
+    <t>: Cek Ketersediaan</t>
+  </si>
+  <si>
     <t>Nama Tester</t>
   </si>
   <si>
+    <t>: Yudistryan Izhar</t>
+  </si>
+  <si>
     <t>NO.</t>
   </si>
   <si>
@@ -53,25 +59,64 @@
     <t>DEFECT ID</t>
   </si>
   <si>
+    <t>NOTE</t>
+  </si>
+  <si>
     <t>#1</t>
   </si>
   <si>
-    <t>Dari dokumen RTM. Langkah-langkah pengujian untuk fitur mau dibuat</t>
-  </si>
-  <si>
-    <t>Dari dokumen RTM</t>
-  </si>
-  <si>
-    <t>hasil yg diharapkan setelah dilakukan uji coba</t>
-  </si>
-  <si>
-    <t>hasil sebenarnya yg keluar setelah dilakukan uji coba</t>
-  </si>
-  <si>
-    <t>status dari hasil uji coba (passed or failed)</t>
-  </si>
-  <si>
-    <t>Jika Failed maka harus disebutkan ID</t>
+    <t>1. Masuk ke halaman Cek Ketersediaan.</t>
+  </si>
+  <si>
+    <t>TC_ck_01</t>
+  </si>
+  <si>
+    <t>- Kota = Bandung
+- Alamat = jl. Kapten Pattimura</t>
+  </si>
+  <si>
+    <t>Pop-up bahwa lokasi tersedia</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Tidak ada masalah dengan fungsi cek ketersediaan dalam situs namun mengaksesnya harus dengan internet kecepatan tinggi. Pada tanggal 19 Desember, pengujian dilakukan menggunakan internet dengan kecepatan up to 10MBps dan beberapa kali terdapat skenario yang gagal, namun pada tanggal 22 Desember saya menggunakan internet dengan kecepatan up to 100MBps dan semua skenario sukses.</t>
+  </si>
+  <si>
+    <t>2. Masukkan lokasi pada elemen "Cari Lokasi".</t>
+  </si>
+  <si>
+    <t>3. Masukkan alamat pada elemen "Alamat".</t>
+  </si>
+  <si>
+    <t>TC_ck_02</t>
+  </si>
+  <si>
+    <t>- Kota = Sibolga
+- Alamat = jl. Yayaya</t>
+  </si>
+  <si>
+    <t>Pop-up bahwa lokasi tidak tersedia</t>
+  </si>
+  <si>
+    <t>4. Klik tombol "Cek Ketersediaan".</t>
+  </si>
+  <si>
+    <t>5. Tunggu sampai web selesai memproses.</t>
+  </si>
+  <si>
+    <t>TC_ck_03</t>
+  </si>
+  <si>
+    <t>- Kota = Mars
+- Alamat = jl. Yayaya</t>
+  </si>
+  <si>
+    <t>6. Muncul pop-up.</t>
   </si>
   <si>
     <t>BUG REPORT</t>
@@ -84,15 +129,6 @@
   </si>
   <si>
     <t>SEVERITY</t>
-  </si>
-  <si>
-    <t>Sesuai yang ada di Test Report</t>
-  </si>
-  <si>
-    <t>prioritaskan defect tersebut termasuk kategori HIGH , MEDIUM or LOW</t>
-  </si>
-  <si>
-    <t>seberapa bahaya defect tersebut (CRITICAL, HIGH, MEDIUM, LOW)</t>
   </si>
 </sst>
 </file>
@@ -171,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border/>
     <border>
       <left/>
@@ -219,6 +255,25 @@
       </top>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -227,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -252,17 +307,28 @@
     <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="2" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -270,10 +336,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,6 +569,7 @@
     <col customWidth="1" min="6" max="6" width="27.71"/>
     <col customWidth="1" min="7" max="7" width="28.14"/>
     <col customWidth="1" min="8" max="8" width="32.86"/>
+    <col customWidth="1" min="9" max="9" width="45.29"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -518,27 +585,25 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" ht="17.25" customHeight="1">
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>2</v>
@@ -547,97 +612,232 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-    </row>
-    <row r="5" ht="19.5" customHeight="1">
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" ht="17.25" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>2</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" ht="19.5" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-    </row>
-    <row r="7" hidden="1">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" ht="42.75" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" hidden="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" ht="42.75" customHeight="1">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" ht="68.25" customHeight="1">
-      <c r="A9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="H9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="I9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="11" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="C10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="D10" s="14" t="s">
         <v>19</v>
       </c>
+      <c r="E10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="15"/>
+      <c r="B11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="15"/>
+      <c r="B12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="15"/>
+      <c r="B13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="15"/>
+      <c r="B14" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="16"/>
+      <c r="B15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
+  <mergeCells count="23">
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I15"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G12:G13"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -664,97 +864,109 @@
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="12"/>
+      <c r="A1" s="17"/>
     </row>
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" ht="17.25" customHeight="1">
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" ht="17.25" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" ht="18.75" customHeight="1">
+    <row r="6" ht="16.5" customHeight="1">
       <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="18"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" ht="1.5" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-    </row>
-    <row r="8" ht="33.0" customHeight="1">
-      <c r="A8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="16" t="s">
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" ht="1.5" customHeight="1">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" ht="33.0" customHeight="1">
+      <c r="A9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" ht="68.25" customHeight="1">
+      <c r="A10" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" ht="68.25" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>26</v>
+      <c r="B10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
   <printOptions/>

</xml_diff>